<commit_message>
petites modifs code industrie
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Industry_model/Input/Steel/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D978EDE9-558C-4184-872E-1CE5FDAE3D1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC9F9C5-24AA-2243-ADE6-3A292AAAEBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="500" windowWidth="21840" windowHeight="11540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="4" r:id="rId1"/>
@@ -22,6 +22,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1227,16 +1235,16 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1280,7 +1288,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +1312,7 @@
       <c r="M2" s="21"/>
       <c r="N2" s="21"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1332,7 +1340,7 @@
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1362,7 @@
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1376,7 +1384,7 @@
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1406,7 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1425,7 +1433,7 @@
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1452,7 +1460,7 @@
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
@@ -1474,7 +1482,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -1518,7 +1526,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1544,7 +1552,7 @@
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -1568,7 +1576,7 @@
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
@@ -1590,7 +1598,7 @@
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -1614,7 +1622,7 @@
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1654,7 +1662,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1701,15 +1709,15 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12"/>
       <c r="B1" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1718,7 +1726,7 @@
         <v>33.333600000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1727,7 +1735,7 @@
         <v>11.666760000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>6.6389420000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1745,7 +1753,7 @@
         <v>4.4444800000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -1767,14 +1775,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="148.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="148.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1785,7 +1793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>40</v>
       </c>
@@ -1793,7 +1801,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>40</v>
       </c>
@@ -1801,7 +1809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
@@ -1809,7 +1817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>40</v>
       </c>
@@ -1817,7 +1825,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>40</v>
       </c>
@@ -1825,7 +1833,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>41</v>
       </c>
@@ -1834,7 +1842,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1842,7 +1850,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1850,7 +1858,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>44</v>
       </c>
@@ -1859,7 +1867,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1867,7 +1875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1875,7 +1883,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>50</v>
       </c>
@@ -1886,7 +1894,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>60</v>
       </c>
@@ -1897,7 +1905,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1924,9 +1932,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9"/>
       <c r="B1" s="10" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
_ modifs données Excel indsutrie
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
@@ -1,42 +1,212 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Industry_model/Input/Steel/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC9F9C5-24AA-2243-ADE6-3A292AAAEBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D857F5F-1325-4C1D-A117-D8E912D2117C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="500" windowWidth="21840" windowHeight="11540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="4" r:id="rId1"/>
-    <sheet name="Conversion table" sheetId="5" r:id="rId2"/>
-    <sheet name="Sources" sheetId="2" r:id="rId3"/>
-    <sheet name="Comment" sheetId="3" r:id="rId4"/>
+    <sheet name="Sources" sheetId="2" r:id="rId2"/>
+    <sheet name="Comment" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Quentin RAILLARD-CAZANOVE</author>
+  </authors>
+  <commentList>
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{D97E1A83-05AF-4173-B39F-B7FEFD319D9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quentin RAILLARD-CAZANOVE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Same assumption as for E_boiler</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{14346994-538D-4008-8EFC-83D237699BC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quentin RAILLARD-CAZANOVE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+calculated from source excluding boiler gas consumption from our own assumptions and assuming all water is consumed for steam generation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{9FFC9D02-F8A3-49D5-82F4-7A61FB65AE27}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quentin RAILLARD-CAZANOVE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1t of steam is equal to about 760kWh of energy. Assuming 100% efficiency for the boiler we have 0,76MWh of electricity consumption</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{AEAB9837-15F6-464D-81E9-925EFA1F63F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quentin RAILLARD-CAZANOVE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+wet manure based biogas
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{A13B7081-E87B-49BE-AFB9-A334043D99E3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quentin RAILLARD-CAZANOVE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Oil (Brent)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{2F8A5B43-A408-4DBE-BCA7-1FD004B89D9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quentin RAILLARD-CAZANOVE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+assuming mass conservation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{E3AEBE38-45D6-4A9F-BBE4-88D5B383C1D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Quentin RAILLARD-CAZANOVE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+assuming mass conservation</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>coal</t>
   </si>
@@ -125,66 +295,12 @@
     <t>to fill</t>
   </si>
   <si>
-    <t>https://france.arcelormittal.com/news/2022/fev/vers-une-production-dacier-sans-co2-en-france.aspx</t>
-  </si>
-  <si>
-    <t>https://france.arcelormittal.com/developpement-durable/co2.aspx</t>
-  </si>
-  <si>
-    <t>https://www.entreprises.gouv.fr/files/files/directions_services/semaine-industrie/img/evenement/presentation_arcelormittal_france_16mars16.pdf</t>
-  </si>
-  <si>
-    <t>https://france.arcelormittal.com/news/2022/mars/arcelormittal-investit-300-millions-deuros-a-mardyck.aspx</t>
-  </si>
-  <si>
-    <t>https://corporate.arcelormittal.com/media/news-articles/arcelormittal-europe-to-produce-green-steel-starting-in-2020</t>
-  </si>
-  <si>
-    <t>10.1016/J.JCLEPRO.2018.08.279</t>
-  </si>
-  <si>
     <t>https://www.eclairerlavenir.fr/rapport-2021-du-groupe-de-travail-n4/</t>
   </si>
   <si>
-    <t>https://www.senat.fr/rap/r18-649-1/r18-649-117.html</t>
-  </si>
-  <si>
-    <t>10.1016/J.JOULE.2021.02.018</t>
-  </si>
-  <si>
-    <t>https://irena.org/-/media/Files/IRENA/Agency/Publication/2020/Dec/IRENA_Green_hydrogen_cost_2020.pdf</t>
-  </si>
-  <si>
-    <t>https://data.jrc.ec.europa.eu/dataset/jrc-10110-10001</t>
-  </si>
-  <si>
-    <t>Arcelor Mittal</t>
-  </si>
-  <si>
-    <t>(Vogl et al, 2018)</t>
-  </si>
-  <si>
     <t>CRE</t>
   </si>
   <si>
-    <t>Sénat</t>
-  </si>
-  <si>
-    <t>(Fan et al, 2021)</t>
-  </si>
-  <si>
-    <t>IRENA</t>
-  </si>
-  <si>
-    <t>JRC-IDEES 2015</t>
-  </si>
-  <si>
-    <t>t to MWh</t>
-  </si>
-  <si>
-    <t>10.1016/J.JCLEPRO.2014.05.063</t>
-  </si>
-  <si>
     <t>costs</t>
   </si>
   <si>
@@ -231,6 +347,81 @@
   </si>
   <si>
     <t>electrolyser consumption</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S095965261400540X</t>
+  </si>
+  <si>
+    <t>Own assumption</t>
+  </si>
+  <si>
+    <t>IEA</t>
+  </si>
+  <si>
+    <t>Biomethane price</t>
+  </si>
+  <si>
+    <t>https://www.iea.org/reports/outlook-for-biogas-and-biomethane-prospects-for-organic-growth/sustainable-supply-potential-and-costs</t>
+  </si>
+  <si>
+    <t>INSIDER</t>
+  </si>
+  <si>
+    <t>Fuel price on 08/08/2022</t>
+  </si>
+  <si>
+    <t>https://markets.businessinsider.com/commodities/coal-price</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0360319920310715</t>
+  </si>
+  <si>
+    <t>(Grigoriev et al, 2020)</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0961953415300891?via%3Dihub</t>
+  </si>
+  <si>
+    <t>(Budsberg et al, 2015)</t>
+  </si>
+  <si>
+    <t>SMR emissions</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0360319921014920</t>
+  </si>
+  <si>
+    <t>water and gas consumption for SMR</t>
+  </si>
+  <si>
+    <t>(Khan et al, 2021)</t>
+  </si>
+  <si>
+    <t>JRC_Biomass</t>
+  </si>
+  <si>
+    <t>biomass/biogas emissions</t>
+  </si>
+  <si>
+    <t>https://publications.jrc.ec.europa.eu/repository/bitstream/JRC104759/ld1a27215enn.pdf</t>
+  </si>
+  <si>
+    <t>energy.gov</t>
+  </si>
+  <si>
+    <t>Coal and gas production LCA</t>
+  </si>
+  <si>
+    <t>https://www.energy.gov/sites/prod/files/2019/09/f66/Life%20Cycle%20Analysis%20of%20Natural%20Gas%20Extraction%20and%20Power%20Generation%2005_29_14%20NETL.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0959652615019241#bib35</t>
+  </si>
+  <si>
+    <t>Oil production emissions</t>
+  </si>
+  <si>
+    <t>(Zhao et al, 2017)</t>
   </si>
 </sst>
 </file>
@@ -241,7 +432,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,8 +456,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,20 +487,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -311,18 +511,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -339,58 +575,57 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
@@ -924,8 +1159,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162A324C-91D6-4E2E-BBB0-429EC5DA63B5}" name="Tableau2" displayName="Tableau2" ref="A1:C1048576" totalsRowShown="0">
-  <autoFilter ref="A1:C1048576" xr:uid="{A4DB52C6-C72E-419E-94E1-402E072AFA9D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{162A324C-91D6-4E2E-BBB0-429EC5DA63B5}" name="Tableau2" displayName="Tableau2" ref="A1:C1048568" totalsRowShown="0">
+  <autoFilter ref="A1:C1048568" xr:uid="{A4DB52C6-C72E-419E-94E1-402E072AFA9D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B00E869B-4749-4997-968B-712B16B60D42}" name="Name"/>
     <tableColumn id="2" xr3:uid="{8A746971-D955-4701-BD9F-9613B6E8A947}" name="About"/>
@@ -1231,712 +1466,663 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0CEE37-33A3-4179-A627-9FAA023AC5EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0CEE37-33A3-4179-A627-9FAA023AC5EF}">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="M1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18">
         <v>-1</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="18">
         <v>-1</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18">
         <v>-1</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="18">
         <v>-1</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4">
+      <c r="I3" s="18"/>
+      <c r="J3" s="28">
         <v>6.7668631583278155E-2</v>
       </c>
-      <c r="K3" s="3">
-        <v>3.04</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="K3" s="35">
+        <f>3.38-0.44</f>
+        <v>2.94</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="18">
         <v>-1</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18">
         <v>-1</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18">
         <v>-1</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18">
         <v>-1</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="18">
         <v>-1</v>
       </c>
-      <c r="K7" s="8">
-        <f>4.9/1.1</f>
-        <v>4.4545454545454541</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="K7" s="36">
+        <v>6.5490000000000004</v>
+      </c>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18">
         <v>-1</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="4">
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="28">
         <f>1/0.99*0.75</f>
         <v>0.75757575757575757</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3">
-        <v>55</v>
-      </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="14">
+        <v>45</v>
+      </c>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="21">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19">
         <v>-1</v>
       </c>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6">
-        <f>29308*0.00001621</f>
-        <v>0.47508267999999998</v>
-      </c>
-      <c r="D10" s="6">
-        <f>0.000001*9*16900</f>
-        <v>0.15210000000000001</v>
-      </c>
-      <c r="E10" s="7">
-        <f>41816*0.0000136</f>
-        <v>0.56869760000000003</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="C10" s="38">
+        <f>29308*0.0000049</f>
+        <v>0.14360919999999999</v>
+      </c>
+      <c r="D10" s="17">
+        <f>0.000001*5*16900</f>
+        <v>8.4499999999999992E-2</v>
+      </c>
+      <c r="E10" s="41">
+        <f>41816*0.000016</f>
+        <v>0.66905599999999998</v>
+      </c>
+      <c r="F10" s="27">
         <v>0.06</v>
       </c>
-      <c r="G10" s="7">
-        <f>45998*0.0000097</f>
-        <v>0.44618060000000004</v>
-      </c>
-      <c r="H10" s="6">
+      <c r="G10" s="39">
+        <f>45998*0.0000084</f>
+        <v>0.38638319999999998</v>
+      </c>
+      <c r="H10" s="17">
         <f>0.000001*-84*14500</f>
         <v>-1.218</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6">
+      <c r="I10" s="22"/>
+      <c r="J10" s="27">
         <f>J3/0.000277778*0.00005624</f>
         <v>1.3700450864516135E-2</v>
       </c>
-      <c r="K10" s="3">
-        <v>12.13</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="21">
+      <c r="K10" s="20"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19">
         <v>-1</v>
       </c>
-      <c r="N10" s="21"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="27">
-        <f>764000000/(607*365)</f>
-        <v>3448.3536819299948</v>
-      </c>
-      <c r="L11" s="17">
-        <f>650000*L8/(8760)</f>
-        <v>4081.0502283105025</v>
-      </c>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="25">
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="10">
+        <f>(764-367)*1000000/(607*365)</f>
+        <v>1791.8801200604817</v>
+      </c>
+      <c r="L11" s="31">
+        <f>1000000*L8/(8760)</f>
+        <v>5136.9863013698632</v>
+      </c>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="9">
         <v>25</v>
       </c>
-      <c r="L12" s="18">
-        <v>10</v>
-      </c>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="1">
+      <c r="L12" s="31">
+        <v>20</v>
+      </c>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="16">
         <v>0.1</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="28">
         <v>0.1</v>
       </c>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="26">
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="28">
         <f>(K13*(1+K13)^K12/((1+K13)^K12-1))</f>
         <v>0.11016807219002084</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="28">
         <f>(L13*(1+L13)^L12/((1+L13)^L12-1))</f>
-        <v>0.16274539488251155</v>
-      </c>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="3" t="s">
+        <v>0.11745962477254576</v>
+      </c>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3">
-        <f>250*0.95</f>
-        <v>237.5</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15" s="26">
+        <v>314</v>
+      </c>
+      <c r="D15" s="16">
         <v>400</v>
       </c>
-      <c r="E15" s="3">
-        <f>60*17.8</f>
-        <v>1068</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15" s="26">
+        <f>94.16/0.138</f>
+        <v>682.31884057971001</v>
+      </c>
+      <c r="F15" s="16">
         <v>60</v>
       </c>
-      <c r="G15" s="3">
-        <v>291.66900000000004</v>
-      </c>
-      <c r="H15" s="3">
-        <f>49.2578*13</f>
-        <v>640.35140000000001</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="27">
+      <c r="G15" s="25">
+        <f>7.83/0.0192</f>
+        <v>407.81250000000006</v>
+      </c>
+      <c r="H15" s="23">
+        <f>16.4/0.02</f>
+        <v>819.99999999999989</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="10">
         <f>(30+39+2+1)*1000000/(607*365)</f>
         <v>324.97573965832413</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="23">
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="16">
         <v>1</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="16">
         <v>1</v>
       </c>
-      <c r="K16" s="3">
-        <v>16.3</v>
-      </c>
-      <c r="L16" s="3">
+      <c r="K16" s="18"/>
+      <c r="L16" s="16">
         <v>9</v>
       </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21">
+      <c r="M16" s="19"/>
+      <c r="N16" s="19">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A79A207-36C8-455B-8B01-DF3AD48E0882}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1196D17-6166-40A9-953F-A236C50591E1}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="148.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="14">
-        <f>0.27778*120</f>
-        <v>33.333600000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="14">
-        <f>0.27778*42</f>
-        <v>11.666760000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="14">
-        <f>0.27778*23.9</f>
-        <v>6.6389420000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="14">
-        <f>0.27778*16</f>
-        <v>4.4444800000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="14">
-        <f>0.27778*42</f>
-        <v>11.666760000000002</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{358BA917-8DA9-428A-ADCE-B506282B9068}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{2854F442-718B-4016-BAA9-DCB2F91D2568}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{4C3D7E32-369A-4B42-866E-A597609780DD}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{CE47F726-CF47-4B8A-8E60-419DB480FF1D}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{71C22888-7BC8-4E2A-83A6-9A209D555548}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1196D17-6166-40A9-953F-A236C50591E1}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="148.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B857DC7-3FA9-4644-A7FC-535374C66D32}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="9"/>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
_ Création d'un nouveau modèle Industry_model_planification.py (incluant un set temporel) et du fichier input associé (parameters_planification.xlsx)   * inclusion évolution temporelle (année par année)   * cas d'étude acier de 2015 à 2030
_ TODO:
  * inclure la planification dans la fonction coût
  * inclure la possibilité de fixer l'implémentation d'une technologie à une année précise (il n'y aura pas de capacité installé avant donc)

_ Excel parameters_planification.xlsx:
  * création d'une nouvelle feuille (TECHNOLOGIES_capacity) dédié à la définition des capacités installées (utile pour donner l'état initial avec notamment la date de mise en marche des unités)
  * Décomposition des technologies par type (e.g pour l'acier DRI-EAF qui peut être avec du CH4 ou de l'H2)
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D857F5F-1325-4C1D-A117-D8E912D2117C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C5ABCB-80FA-4AE3-8B5C-43B5C9B5010B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Quentin RAILLARD-CAZANOVE:</t>
         </r>
@@ -49,7 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Same assumption as for E_boiler</t>
@@ -64,7 +64,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Quentin RAILLARD-CAZANOVE:</t>
         </r>
@@ -73,7 +73,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 calculated from source excluding boiler gas consumption from our own assumptions and assuming all water is consumed for steam generation</t>
@@ -88,7 +88,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Quentin RAILLARD-CAZANOVE:</t>
         </r>
@@ -97,7 +97,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 1t of steam is equal to about 760kWh of energy. Assuming 100% efficiency for the boiler we have 0,76MWh of electricity consumption</t>
@@ -112,7 +112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Quentin RAILLARD-CAZANOVE:</t>
         </r>
@@ -121,7 +121,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 wet manure based biogas
@@ -137,7 +137,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Quentin RAILLARD-CAZANOVE:</t>
         </r>
@@ -146,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Oil (Brent)</t>
@@ -161,7 +161,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Quentin RAILLARD-CAZANOVE:</t>
         </r>
@@ -170,7 +170,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 assuming mass conservation</t>
@@ -185,7 +185,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Quentin RAILLARD-CAZANOVE:</t>
         </r>
@@ -194,7 +194,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 assuming mass conservation</t>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="74">
   <si>
     <t>coal</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t>(Zhao et al, 2017)</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0306261921014215</t>
+  </si>
+  <si>
+    <t>(Longden et al, 2022)</t>
   </si>
 </sst>
 </file>
@@ -468,14 +474,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1469,17 +1475,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0CEE37-33A3-4179-A627-9FAA023AC5EF}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1523,7 +1529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
@@ -1547,7 +1553,7 @@
       <c r="M2" s="19"/>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
@@ -1576,7 +1582,7 @@
       <c r="M3" s="19"/>
       <c r="N3" s="19"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1604,7 @@
       <c r="M4" s="19"/>
       <c r="N4" s="19"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
@@ -1620,7 +1626,7 @@
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
@@ -1642,7 +1648,7 @@
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
@@ -1668,7 +1674,7 @@
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
@@ -1695,7 +1701,7 @@
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>39</v>
       </c>
@@ -1717,7 +1723,7 @@
       </c>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>14</v>
       </c>
@@ -1752,14 +1758,17 @@
         <f>J3/0.000277778*0.00005624</f>
         <v>1.3700450864516135E-2</v>
       </c>
-      <c r="K10" s="20"/>
+      <c r="K10" s="18">
+        <f>0.18*11.67*(K3)</f>
+        <v>6.175764</v>
+      </c>
       <c r="L10" s="18"/>
       <c r="M10" s="19">
         <v>-1</v>
       </c>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>33</v>
       </c>
@@ -1785,7 +1794,7 @@
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>35</v>
       </c>
@@ -1809,7 +1818,7 @@
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>38</v>
       </c>
@@ -1831,7 +1840,7 @@
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>37</v>
       </c>
@@ -1855,7 +1864,7 @@
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>34</v>
       </c>
@@ -1895,7 +1904,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>13</v>
       </c>
@@ -1935,20 +1944,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1196D17-6166-40A9-953F-A236C50591E1}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="148.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="148.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1959,14 +1968,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1974,7 +1983,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>63</v>
       </c>
@@ -1985,7 +1994,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -1996,7 +2005,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>42</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>45</v>
       </c>
@@ -2018,7 +2027,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>49</v>
       </c>
@@ -2029,7 +2038,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2049,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>56</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>58</v>
       </c>
@@ -2062,7 +2071,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
@@ -2073,7 +2082,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>66</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="40" t="s">
         <v>71</v>
       </c>
@@ -2093,6 +2102,17 @@
       </c>
       <c r="C14" s="40" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2118,9 +2138,9 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
_ MaJ n°2 du modèle Europe 7 noeuds  * Données pour 2017-2019 (à mettre à jour pour les coûts) et 2030  * Notebooks pour extraction et analyse des résultats  * Les données étaient incompletes --> elles ont été completées
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/Resources_Technologies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickdartois/Documents/Corps des Mines/3A/Mémoire 3A/Modèle/Energy-Alternatives-Planing/Models/Industry_model/Input/Steel/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C43E064-3FCD-1246-8AF6-2665FADA3AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958730F3-1F3B-412C-93C2-9CBEA6BF3B63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23860" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23856" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="4" r:id="rId1"/>
@@ -29,8 +29,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1240,13 +1240,13 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1314,7 +1314,7 @@
       <c r="M2" s="21"/>
       <c r="N2" s="21"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1408,7 +1408,7 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1435,7 +1435,7 @@
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -1624,7 +1624,7 @@
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1711,15 +1711,15 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>33.333600000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>11.666760000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>6.6389420000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>4.4444800000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -1777,14 +1777,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="148.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="148.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>40</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>40</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>40</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>40</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>41</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>44</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>50</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>60</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1934,9 +1934,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="B1" s="10" t="s">
         <v>28</v>

</xml_diff>